<commit_message>
C3 1.1 replace C13 to be 4.7uF
</commit_message>
<xml_diff>
--- a/Hardware/C3-27-epaper-touch/production/C3-BOM.xlsx
+++ b/Hardware/C3-27-epaper-touch/production/C3-BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12" count="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11" count="11">
   <si>
     <t>C_0805_2012Metric_Pad1.18x1.45mm_HandSolder</t>
   </si>
@@ -52,9 +52,6 @@
   </si>
   <si>
     <t>AFC24-S24FIC-00</t>
-  </si>
-  <si>
-    <t>C31850</t>
   </si>
 </sst>
 </file>
@@ -134,7 +131,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -597,15 +594,11 @@
       <c r="B23" t="s">
         <v>9</v>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>100nF</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>C28233</t>
-        </is>
+      <c r="C23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="13.5">
@@ -826,8 +819,10 @@
           <t>22K</t>
         </is>
       </c>
-      <c r="D34" t="s">
-        <v>11</v>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>C31850</t>
+        </is>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13.5">

</xml_diff>